<commit_message>
add complete table results
</commit_message>
<xml_diff>
--- a/bests-results-all_metrics.xlsx
+++ b/bests-results-all_metrics.xlsx
@@ -18,15 +18,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="29">
   <si>
     <t>BoW (TFIDF)</t>
   </si>
   <si>
-    <t>precisão</t>
+    <t>precision</t>
   </si>
   <si>
-    <t>revocação</t>
+    <t>recall</t>
   </si>
   <si>
     <t>f1-score</t>
@@ -35,13 +35,13 @@
     <t>auc_roc</t>
   </si>
   <si>
-    <t xml:space="preserve">acuracia </t>
+    <t xml:space="preserve">accuracy </t>
   </si>
   <si>
-    <t>média</t>
+    <t>mean</t>
   </si>
   <si>
-    <t>desvio padrão</t>
+    <t>std</t>
   </si>
   <si>
     <t>3_%</t>
@@ -65,7 +65,7 @@
     <t>DistilBERT</t>
   </si>
   <si>
-    <t>InfDensidade</t>
+    <t>Density</t>
   </si>
   <si>
     <t>Features LIWK</t>
@@ -77,16 +77,13 @@
     <t>VAE</t>
   </si>
   <si>
-    <t>MVAE (Densidade)</t>
+    <t>MVAE -FakeNews</t>
   </si>
   <si>
-    <t>MVAE (Liwk)</t>
+    <t>MVAE -LIWC</t>
   </si>
   <si>
     <t>FakeBr</t>
-  </si>
-  <si>
-    <t>infDensidade</t>
   </si>
   <si>
     <t>Autoencoder</t>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>FNN</t>
-  </si>
-  <si>
-    <t>BoW</t>
   </si>
   <si>
     <t>FCN</t>
@@ -121,7 +115,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -141,6 +135,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -153,6 +156,10 @@
     <font>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <name val="Arial"/>
     </font>
     <font>
@@ -270,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -288,107 +295,110 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="10" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -7398,8 +7408,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
+      <c r="A7" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="B7" s="15">
         <v>0.621405657963184</v>
@@ -7413,13 +7423,13 @@
       <c r="E7" s="15">
         <v>0.01871290325052</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="27">
         <v>0.646482372114214</v>
       </c>
       <c r="G7" s="15">
         <v>0.019403635575743</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="27">
         <v>0.649782742159112</v>
       </c>
       <c r="I7" s="15">
@@ -7427,7 +7437,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="16">
@@ -7457,7 +7467,7 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="15">
         <v>0.622314735533477</v>
@@ -7515,15 +7525,15 @@
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="26">
+        <v>23</v>
+      </c>
+      <c r="B11" s="27">
         <v>0.642299509286765</v>
       </c>
       <c r="C11" s="15">
         <v>0.002744548894172</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="27">
         <v>0.643657026832733</v>
       </c>
       <c r="E11" s="15">
@@ -7544,7 +7554,7 @@
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="15">
         <v>0.636975206265161</v>
@@ -7572,25 +7582,25 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
     </row>
     <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
+      <c r="A14" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>8</v>
@@ -7608,7 +7618,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="32"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15">
       <c r="A15" s="6"/>
@@ -7638,8 +7648,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="25" t="s">
-        <v>27</v>
+      <c r="A16" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="B16" s="15">
         <v>0.001171113327861</v>
@@ -7754,8 +7764,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>22</v>
+      <c r="A20" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="B20" s="15">
         <v>0.324840455197577</v>
@@ -7783,7 +7793,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="16">
@@ -7810,11 +7820,11 @@
       <c r="I21" s="15">
         <v>0.0039137247671</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="15">
         <v>0.336976795790522</v>
@@ -7840,7 +7850,7 @@
       <c r="I22" s="15">
         <v>0.004845466299575</v>
       </c>
-      <c r="J22" s="32"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
@@ -7870,45 +7880,45 @@
       <c r="I23" s="15">
         <v>0.003640768848949</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
     </row>
     <row r="24">
       <c r="A24" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="26">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27">
         <v>0.395365891025642</v>
       </c>
       <c r="C24" s="15">
         <v>0.025125621583281</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="27">
         <v>0.403442110221692</v>
       </c>
       <c r="E24" s="15">
         <v>0.030436211382313</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="27">
         <v>0.396564285255236</v>
       </c>
       <c r="G24" s="15">
         <v>0.014235074726233</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="27">
         <v>0.393257829150128</v>
       </c>
       <c r="I24" s="15">
         <v>0.014726798183489</v>
       </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
     </row>
     <row r="25">
       <c r="A25" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="15">
         <v>0.385753814954236</v>
@@ -7928,47 +7938,47 @@
       <c r="G25" s="15">
         <v>0.004289766383867</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="27">
         <v>0.393279604992048</v>
       </c>
       <c r="I25" s="15">
         <v>0.003410974803661</v>
       </c>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
     </row>
     <row r="27">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
+      <c r="A28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>8</v>
@@ -7986,9 +7996,9 @@
         <v>11</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
     </row>
     <row r="29">
       <c r="A29" s="6"/>
@@ -8018,8 +8028,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="25" t="s">
-        <v>27</v>
+      <c r="A30" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="B30" s="15">
         <v>4.24854076275E-4</v>
@@ -8134,8 +8144,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="25" t="s">
-        <v>22</v>
+      <c r="A34" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="B34" s="15">
         <v>0.486670167567474</v>
@@ -8163,7 +8173,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="16">
@@ -8193,7 +8203,7 @@
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="15">
         <v>0.374643491857762</v>
@@ -8251,27 +8261,27 @@
     </row>
     <row r="38">
       <c r="A38" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="26">
+        <v>23</v>
+      </c>
+      <c r="B38" s="27">
         <v>0.805400065313175</v>
       </c>
       <c r="C38" s="15">
         <v>0.022479826980877</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="27">
         <v>0.812670151817844</v>
       </c>
       <c r="E38" s="15">
         <v>0.030406006962706</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="27">
         <v>0.811089870207598</v>
       </c>
       <c r="G38" s="15">
         <v>0.015563821123585</v>
       </c>
-      <c r="H38" s="26">
+      <c r="H38" s="27">
         <v>0.80778642676259</v>
       </c>
       <c r="I38" s="15">
@@ -8280,7 +8290,7 @@
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="15">
         <v>0.725888013467116</v>
@@ -8340,7 +8350,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -8361,7 +8371,7 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
@@ -8391,34 +8401,34 @@
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="37">
         <v>0.624403296463841</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="38">
         <v>0.034095749270089</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="37">
         <v>0.60313536818435</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="38">
         <v>0.02660000554831</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="37">
         <v>0.593865511397893</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="38">
         <v>0.016282694691066</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="37">
         <v>0.578069260682201</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="38">
         <v>0.011267646894455</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="13">
         <v>0.474118044509644</v>
@@ -8447,7 +8457,7 @@
     </row>
     <row r="5">
       <c r="A5" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="13">
         <v>0.472952567971373</v>
@@ -8478,62 +8488,62 @@
       <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="39">
         <v>0.539486267102854</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="39">
         <v>0.006165576834426</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="39">
         <v>0.52792694741653</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="39">
         <v>0.003659841452823</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="39">
         <v>0.520950186492849</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="39">
         <v>0.003258438284176</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="39">
         <v>0.512480531440713</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="39">
         <v>0.003187670892091</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="38">
+      <c r="A7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39">
         <v>0.50630653656011</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="39">
         <v>0.019121736352724</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="39">
         <v>0.500849016262678</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="39">
         <v>0.012469078420579</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="39">
         <v>0.517187248270901</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="39">
         <v>0.012888196061717</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="39">
         <v>0.516409285422021</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="39">
         <v>0.012660694782036</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="16">
@@ -8563,30 +8573,30 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="38">
+        <v>22</v>
+      </c>
+      <c r="B9" s="39">
         <v>0.501445682676248</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="39">
         <v>0.004032977486256</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="39">
         <v>0.48751790206177</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="39">
         <v>0.003361304086127</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="39">
         <v>0.481259053660931</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="39">
         <v>0.002239824809492</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="39">
         <v>0.480136504054713</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="39">
         <v>0.001878415700838</v>
       </c>
     </row>
@@ -8594,103 +8604,103 @@
       <c r="A10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="39">
         <v>0.48381145387825</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="39">
         <v>0.003646417387296</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="39">
         <v>0.483313297137934</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="39">
         <v>0.004028182762504</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="39">
         <v>0.483427420844538</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="39">
         <v>0.00219004798708</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="39">
         <v>0.483470923623027</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="39">
         <v>0.003429108945601</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="38">
+        <v>23</v>
+      </c>
+      <c r="B11" s="39">
         <v>0.477372204550997</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="39">
         <v>0.003375024100434</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="39">
         <v>0.479579455410718</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="39">
         <v>0.005078248052027</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="39">
         <v>0.48293576417049</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="39">
         <v>0.004928302480563</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="39">
         <v>0.484747128235039</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="39">
         <v>0.005150231213811</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="39">
+        <v>0.474349449599306</v>
+      </c>
+      <c r="C12" s="39">
+        <v>0.002744560363109</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0.474404883625932</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.002483265630806</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.485103021008284</v>
+      </c>
+      <c r="G12" s="39">
+        <v>0.004254345467393</v>
+      </c>
+      <c r="H12" s="39">
+        <v>0.481205390921118</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.004605631316399</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="32" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="38">
-        <v>0.474349449599306</v>
-      </c>
-      <c r="C12" s="38">
-        <v>0.002744560363109</v>
-      </c>
-      <c r="D12" s="38">
-        <v>0.474404883625932</v>
-      </c>
-      <c r="E12" s="38">
-        <v>0.002483265630806</v>
-      </c>
-      <c r="F12" s="38">
-        <v>0.485103021008284</v>
-      </c>
-      <c r="G12" s="38">
-        <v>0.004254345467393</v>
-      </c>
-      <c r="H12" s="38">
-        <v>0.481205390921118</v>
-      </c>
-      <c r="I12" s="38">
-        <v>0.004605631316399</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>8</v>
@@ -8737,37 +8747,37 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="39">
+      <c r="A16" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="40">
         <v>0.416666666666667</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="39">
         <v>0.442530601578392</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="40">
         <v>0.563037717412139</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="39">
         <v>0.06488939112177</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="40">
         <v>0.483264958469039</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="39">
         <v>0.026407604262511</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="40">
         <v>0.456277991412212</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="39">
         <v>0.022910840021147</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="13">
         <v>0.219452060175337</v>
@@ -8796,7 +8806,7 @@
     </row>
     <row r="18">
       <c r="A18" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="13">
         <v>0.228372992085901</v>
@@ -8827,62 +8837,62 @@
       <c r="A19" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="39">
         <v>0.2521398726706</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="39">
         <v>0.00988888716619</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="39">
         <v>0.244134511518415</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="39">
         <v>0.007279312683187</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="39">
         <v>0.241411949385392</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="39">
         <v>0.005763010923115</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="39">
         <v>0.240201184714771</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="39">
         <v>0.004985240814754</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="38">
+      <c r="A20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="39">
         <v>0.209201986184996</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="39">
         <v>0.018089548167737</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="39">
         <v>0.222467511929197</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="39">
         <v>0.02926459274678</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="39">
         <v>0.225566968659978</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="39">
         <v>0.010248438111181</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="39">
         <v>0.227375981796201</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="39">
         <v>0.010237880430038</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="16">
@@ -8897,10 +8907,10 @@
       <c r="E21" s="16">
         <v>0.004634589112503</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="39">
         <v>0.263083238617212</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="39">
         <v>0.005711604278193</v>
       </c>
       <c r="H21" s="15">
@@ -8912,18 +8922,18 @@
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="38">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39">
         <v>0.23899922194232</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="39">
         <v>0.00703643703397</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="39">
         <v>0.230477979917016</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="39">
         <v>0.004302815358913</v>
       </c>
       <c r="F22" s="16">
@@ -8932,10 +8942,10 @@
       <c r="G22" s="16">
         <v>0.004712249941228</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="39">
         <v>0.232270845340408</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="39">
         <v>0.003334757890031</v>
       </c>
     </row>
@@ -8943,114 +8953,114 @@
       <c r="A23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="39">
         <v>0.232740301764233</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>0.010163593061854</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="39">
         <v>0.232988089193901</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="39">
         <v>0.0058411438089</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="39">
         <v>0.230832829322818</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="39">
         <v>0.005390714043385</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="39">
         <v>0.228160417512446</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="39">
         <v>0.003108782818692</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="38">
+        <v>23</v>
+      </c>
+      <c r="B24" s="39">
         <v>0.298956106406281</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="39">
         <v>0.031226645803022</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="39">
         <v>0.289078790380316</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="39">
         <v>0.026256692271081</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="39">
         <v>0.273018904562572</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="39">
         <v>0.022984660703407</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="39">
         <v>0.265332432062986</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="39">
         <v>0.013600953407255</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="38">
+        <v>24</v>
+      </c>
+      <c r="B25" s="39">
         <v>0.274993090137387</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="39">
         <v>0.006868768599884</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="39">
         <v>0.262212762822176</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="39">
         <v>0.006687793368224</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="39">
         <v>0.266211644237976</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="39">
         <v>0.007954992474516</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="39">
         <v>0.269901454432688</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="39">
         <v>0.006373134229125</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="33"/>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
+      <c r="A28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>8</v>
@@ -9097,37 +9107,37 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="38">
+      <c r="A30" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="39">
         <v>0.15</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="39">
         <v>0.320156211871642</v>
       </c>
-      <c r="D30" s="39">
+      <c r="D30" s="40">
         <v>0.965909090909091</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="39">
         <v>0.076904201434948</v>
       </c>
-      <c r="F30" s="39">
+      <c r="F30" s="40">
         <v>0.9402628579997</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="39">
         <v>0.042479263519891</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="40">
         <v>0.921346212579544</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="39">
         <v>0.027315410835058</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="13">
         <v>0.505194676854521</v>
@@ -9156,7 +9166,7 @@
     </row>
     <row r="32">
       <c r="A32" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="13">
         <v>0.476132008187072</v>
@@ -9187,62 +9197,62 @@
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="39">
+      <c r="B33" s="40">
         <v>0.922012792459423</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="39">
         <v>0.008266561976423</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="39">
         <v>0.897006953077155</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="39">
         <v>0.017305700400476</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="39">
         <v>0.876702865820489</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="39">
         <v>0.016625412875605</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="39">
         <v>0.852282252873277</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="39">
         <v>0.018725968716607</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="38">
+      <c r="A34" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="39">
         <v>0.486907784551907</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="39">
         <v>0.053385390107326</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="39">
         <v>0.526979772437654</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="39">
         <v>0.062745269905055</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="39">
         <v>0.488905450929903</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="39">
         <v>0.041684374408264</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="39">
         <v>0.514616482970155</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="39">
         <v>0.019944361946465</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="16">
@@ -9272,30 +9282,30 @@
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="38">
+        <v>22</v>
+      </c>
+      <c r="B36" s="39">
         <v>0.851881145510051</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="39">
         <v>0.042235331380298</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="39">
         <v>0.724669722739895</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="39">
         <v>0.048527174045874</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="39">
         <v>0.703817306092951</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="39">
         <v>0.038691959510313</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="39">
         <v>0.760973069382084</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="39">
         <v>0.03409511407298</v>
       </c>
     </row>
@@ -9303,86 +9313,86 @@
       <c r="A37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="39">
         <v>0.833868809139978</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="39">
         <v>0.033878922410089</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="39">
         <v>0.777486379048894</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="39">
         <v>0.036759151032142</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="39">
         <v>0.750599787839797</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="39">
         <v>0.028576084680658</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="39">
         <v>0.728031112535331</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="39">
         <v>0.048163382678633</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="38">
+        <v>23</v>
+      </c>
+      <c r="B38" s="39">
         <v>0.817424066787935</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="39">
         <v>0.039908186993434</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D38" s="39">
         <v>0.796258024616141</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="39">
         <v>0.028736483170771</v>
       </c>
-      <c r="F38" s="38">
+      <c r="F38" s="39">
         <v>0.736834241047707</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="39">
         <v>0.034687279405108</v>
       </c>
-      <c r="H38" s="38">
+      <c r="H38" s="39">
         <v>0.731314155608233</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="39">
         <v>0.031254066528108</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="38">
+        <v>24</v>
+      </c>
+      <c r="B39" s="39">
         <v>0.654262232073286</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="39">
         <v>0.066341026663645</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="39">
         <v>0.687736260335984</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="39">
         <v>0.050610496246209</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="39">
         <v>0.679978412672519</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="39">
         <v>0.059245003344873</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="39">
         <v>0.670691982009444</v>
       </c>
-      <c r="I39" s="38">
+      <c r="I39" s="39">
         <v>0.067318576372171</v>
       </c>
     </row>
@@ -9419,7 +9429,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -9440,7 +9450,7 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
@@ -9470,34 +9480,34 @@
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="38">
         <v>0.01500838777553</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="38">
         <v>0.002884567059545</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="38">
         <v>0.055802601516684</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="38">
         <v>0.006856879711708</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="38">
         <v>0.1074358960179</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="38">
         <v>0.008642995752193</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="38">
         <v>0.170186954811276</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="38">
         <v>0.009007279973076</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="13">
         <v>0.816103508792338</v>
@@ -9526,7 +9536,7 @@
     </row>
     <row r="5">
       <c r="A5" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="13">
         <v>0.889106170340208</v>
@@ -9557,62 +9567,62 @@
       <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="39">
         <v>0.612900650484054</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="39">
         <v>0.019835575193935</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="39">
         <v>0.699800417281583</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="39">
         <v>0.025823134433917</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="39">
         <v>0.75943242877828</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="39">
         <v>0.024098986670637</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="39">
         <v>0.811590729186312</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="39">
         <v>0.026757810122824</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="38">
+      <c r="A7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39">
         <v>0.808161075801578</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="39">
         <v>0.069886533199311</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="39">
         <v>0.861371161498575</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="39">
         <v>0.055967957349165</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="39">
         <v>0.863161570658404</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="39">
         <v>0.044581267905808</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="39">
         <v>0.878233393548859</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="39">
         <v>0.039628157613794</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="16">
@@ -9642,30 +9652,30 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="38">
+        <v>22</v>
+      </c>
+      <c r="B9" s="39">
         <v>0.820330367942736</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="39">
         <v>0.022065567465362</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="39">
         <v>0.908960817827661</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="39">
         <v>0.014019910035443</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="39">
         <v>0.945987759969077</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="39">
         <v>0.010038359879089</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="39">
         <v>0.959637379596757</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="39">
         <v>0.007257378838099</v>
       </c>
     </row>
@@ -9673,103 +9683,103 @@
       <c r="A10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="39">
         <v>0.911678888072921</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="39">
         <v>0.024977431972895</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="39">
         <v>0.9328629269475</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="39">
         <v>0.01569985923968</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="39">
         <v>0.934005493196815</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="39">
         <v>0.017257666362011</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="39">
         <v>0.936692489484531</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="39">
         <v>0.019670568205198</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="39">
+        <v>23</v>
+      </c>
+      <c r="B11" s="40">
         <v>0.981563350922522</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="39">
         <v>0.013026954637627</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="40">
         <v>0.978537830612511</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="39">
         <v>0.009961141841605</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="40">
         <v>0.969303859444643</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="39">
         <v>0.013134486956379</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="40">
         <v>0.967173372087901</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="39">
         <v>0.013787736447955</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="39">
+        <v>0.969427916904481</v>
+      </c>
+      <c r="C12" s="39">
+        <v>0.011194897517615</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0.963252389758008</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.013324915896955</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.928633722232954</v>
+      </c>
+      <c r="G12" s="39">
+        <v>0.011712489042742</v>
+      </c>
+      <c r="H12" s="39">
+        <v>0.951918356823618</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.010070249524241</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="32" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="38">
-        <v>0.969427916904481</v>
-      </c>
-      <c r="C12" s="38">
-        <v>0.011194897517615</v>
-      </c>
-      <c r="D12" s="38">
-        <v>0.963252389758008</v>
-      </c>
-      <c r="E12" s="38">
-        <v>0.013324915896955</v>
-      </c>
-      <c r="F12" s="38">
-        <v>0.928633722232954</v>
-      </c>
-      <c r="G12" s="38">
-        <v>0.011712489042742</v>
-      </c>
-      <c r="H12" s="38">
-        <v>0.951918356823618</v>
-      </c>
-      <c r="I12" s="38">
-        <v>0.010070249524241</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>8</v>
@@ -9819,34 +9829,34 @@
       <c r="A16" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="39">
         <v>5.86531560418E-4</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="39">
         <v>6.14794240694E-4</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="39">
         <v>0.01348984367369</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="39">
         <v>0.003374235216049</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="39">
         <v>0.044444279289418</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="39">
         <v>0.00453862637867</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="39">
         <v>0.104659934004052</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="39">
         <v>0.010756998363028</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="13">
         <v>0.646338966063473</v>
@@ -9875,7 +9885,7 @@
     </row>
     <row r="18">
       <c r="A18" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="13">
         <v>0.799414062997677</v>
@@ -9906,62 +9916,62 @@
       <c r="A19" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="39">
         <v>0.446009878158059</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="39">
         <v>0.052019031685298</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="39">
         <v>0.594071406427173</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="39">
         <v>0.052546110226475</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="39">
         <v>0.664063804577248</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="39">
         <v>0.038863116307013</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="39">
         <v>0.742982006123948</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="39">
         <v>0.03570445320939</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="38">
+      <c r="A20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="39">
         <v>0.736083348551189</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="39">
         <v>0.081454501035586</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="39">
         <v>0.778369891578085</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="39">
         <v>0.05991636958959</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="39">
         <v>0.82014303369021</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="39">
         <v>0.074788975848074</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="39">
         <v>0.828025557504385</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="39">
         <v>0.068082744363895</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="16">
@@ -9982,156 +9992,156 @@
       <c r="G21" s="16">
         <v>0.042448583207425</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="39">
         <v>0.67762108812625</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="39">
         <v>0.030854887862419</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="38">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39">
         <v>0.576276155247612</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="39">
         <v>0.057841779584715</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="39">
         <v>0.759925213085374</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="39">
         <v>0.04364426006603</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="39">
         <v>0.8344735825098</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="39">
         <v>0.020164781334837</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="39">
         <v>0.822877788583635</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="39">
         <v>0.025806521683232</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="39">
+      <c r="B23" s="40">
         <v>0.85467815296281</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>0.034460823097486</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="40">
         <v>0.866476988478314</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="39">
         <v>0.03607599086417</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="40">
         <v>0.902640135219498</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="39">
         <v>0.032997150339147</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="40">
         <v>0.937051076787178</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="39">
         <v>0.020427445577159</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="38">
+        <v>23</v>
+      </c>
+      <c r="B24" s="39">
         <v>0.60614352632406</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="39">
         <v>0.09570188900301</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="39">
         <v>0.675730648195729</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="39">
         <v>0.071389632786901</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="39">
         <v>0.747350946409081</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="39">
         <v>0.094410104499663</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="39">
         <v>0.766445986520518</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="39">
         <v>0.064918237987708</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="38">
+        <v>24</v>
+      </c>
+      <c r="B25" s="39">
         <v>0.653120750502189</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="39">
         <v>0.066761790960238</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="39">
         <v>0.746304226883369</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="39">
         <v>0.044703756674754</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="39">
         <v>0.736337054983883</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="39">
         <v>0.055236397604494</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="39">
         <v>0.727800474797107</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="39">
         <v>0.041581950311629</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="33"/>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
+      <c r="A28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>8</v>
@@ -10181,34 +10191,34 @@
       <c r="A30" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="39">
         <v>2.12765957447E-4</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="39">
         <v>4.25531914894E-4</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="39">
         <v>0.005215031835588</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="39">
         <v>0.002711582129837</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="39">
         <v>0.018945007137516</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="39">
         <v>0.005057921131784</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="39">
         <v>0.058643871932568</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="39">
         <v>0.01286696349971</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="13">
         <v>0.625279269480887</v>
@@ -10237,7 +10247,7 @@
     </row>
     <row r="32">
       <c r="A32" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="13">
         <v>0.780772211270478</v>
@@ -10268,62 +10278,62 @@
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="39">
         <v>0.279056941517685</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="39">
         <v>0.048675559553806</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="39">
         <v>0.417954818389867</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="39">
         <v>0.051594421546458</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="39">
         <v>0.505114426846124</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="39">
         <v>0.040229048221651</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="39">
         <v>0.603882922076451</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="39">
         <v>0.033118547309638</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="38">
+      <c r="A34" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="39">
         <v>0.493518908753087</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="39">
         <v>0.09722872603549</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="39">
         <v>0.64762400018127</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="39">
         <v>0.147051052496946</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="39">
         <v>0.731592005981918</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="39">
         <v>0.107694934603933</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="39">
         <v>0.804511589966692</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="39">
         <v>0.08719047847529</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="16">
@@ -10353,30 +10363,30 @@
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="38">
+        <v>22</v>
+      </c>
+      <c r="B36" s="39">
         <v>0.24288163052591</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="39">
         <v>0.052869474072654</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="39">
         <v>0.56535415675345</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="39">
         <v>0.068158963760364</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="39">
         <v>0.694343348514717</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="39">
         <v>0.031900771745034</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="39">
         <v>0.689135227607459</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="39">
         <v>0.040564130378359</v>
       </c>
     </row>
@@ -10384,86 +10394,86 @@
       <c r="A37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="39">
         <v>0.669882287630571</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="39">
         <v>0.05631182131918</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="39">
         <v>0.818220379308001</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="39">
         <v>0.045470715890647</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="39">
         <v>0.861219155733805</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="39">
         <v>0.037101466727692</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="39">
         <v>0.90123626311377</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="39">
         <v>0.025075366890759</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="38">
+        <v>23</v>
+      </c>
+      <c r="B38" s="39">
         <v>0.797772301905604</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="39">
         <v>0.050488223961793</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="40">
         <v>0.83258865248227</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="39">
         <v>0.056849344615827</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="40">
         <v>0.904747241293363</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="39">
         <v>0.030795600567892</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="40">
         <v>0.903791720481272</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="39">
         <v>0.020877189254384</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="39">
+        <v>24</v>
+      </c>
+      <c r="B39" s="40">
         <v>0.828977409194934</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="39">
         <v>0.073291160573795</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="39">
         <v>0.79833152063082</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="39">
         <v>0.04681039882391</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="39">
         <v>0.840464844900641</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="39">
         <v>0.04009495203272</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="39">
         <v>0.866868103233408</v>
       </c>
-      <c r="I39" s="38">
+      <c r="I39" s="39">
         <v>0.038673683757223</v>
       </c>
     </row>
@@ -10500,7 +10510,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -10521,7 +10531,7 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
@@ -10551,34 +10561,34 @@
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="38">
         <v>0.579126849709491</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="38">
         <v>0.011414536770659</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="38">
         <v>0.577823328521557</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="38">
         <v>0.007858772797863</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="38">
         <v>0.578167816956668</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="38">
         <v>0.00656692900537</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="38">
         <v>0.573216525352696</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="38">
         <v>0.004928888854024</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="13">
         <v>0.508798107232523</v>
@@ -10607,7 +10617,7 @@
     </row>
     <row r="5">
       <c r="A5" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="13">
         <v>0.499317365397346</v>
@@ -10638,62 +10648,62 @@
       <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="39">
         <v>0.600870410333292</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="39">
         <v>0.006603694881835</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="39">
         <v>0.600887957989072</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="39">
         <v>0.005927919597925</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="39">
         <v>0.600922236542349</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="39">
         <v>0.004717599487383</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="39">
         <v>0.600364278741061</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="39">
         <v>0.005012639767601</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="38">
+      <c r="A7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39">
         <v>0.562691561569721</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="39">
         <v>0.039617930454787</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="39">
         <v>0.580702468613456</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="39">
         <v>0.03222327611525</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="39">
         <v>0.583969346140725</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="39">
         <v>0.042839465294807</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="39">
         <v>0.577015693008073</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="39">
         <v>0.020751959032308</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="16">
@@ -10723,30 +10733,30 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="38">
+        <v>22</v>
+      </c>
+      <c r="B9" s="39">
         <v>0.598744412193639</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="39">
         <v>0.010251595319375</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="39">
         <v>0.600501782174907</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="39">
         <v>0.005343451411285</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="39">
         <v>0.601011385719256</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="39">
         <v>0.010064558235885</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="39">
         <v>0.6026329116661</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="39">
         <v>0.008105528983156</v>
       </c>
     </row>
@@ -10754,103 +10764,103 @@
       <c r="A10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="39">
         <v>0.596175149073358</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="39">
         <v>0.007803280417174</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="39">
         <v>0.595290444604902</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="39">
         <v>0.005867324378111</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="39">
         <v>0.595641846349635</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="39">
         <v>0.010986002863281</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="39">
         <v>0.593000536410169</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="39">
         <v>0.009744448628748</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="39">
+        <v>23</v>
+      </c>
+      <c r="B11" s="40">
         <v>0.611461678576731</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="39">
         <v>0.015467049954046</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="40">
         <v>0.621837739886592</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="39">
         <v>0.010394668037134</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="40">
         <v>0.625077532106291</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="39">
         <v>0.015469902923867</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="40">
         <v>0.623933921246329</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="39">
         <v>0.020317260111075</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="40">
+        <v>0.615462469808743</v>
+      </c>
+      <c r="C12" s="39">
+        <v>0.012480234147835</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0.611385063707319</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.013820189129997</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.614235099914897</v>
+      </c>
+      <c r="G12" s="39">
+        <v>0.018105898180975</v>
+      </c>
+      <c r="H12" s="39">
+        <v>0.616470546886727</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.018014897258063</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="32" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="39">
-        <v>0.615462469808743</v>
-      </c>
-      <c r="C12" s="38">
-        <v>0.012480234147835</v>
-      </c>
-      <c r="D12" s="38">
-        <v>0.611385063707319</v>
-      </c>
-      <c r="E12" s="38">
-        <v>0.013820189129997</v>
-      </c>
-      <c r="F12" s="38">
-        <v>0.614235099914897</v>
-      </c>
-      <c r="G12" s="38">
-        <v>0.018105898180975</v>
-      </c>
-      <c r="H12" s="38">
-        <v>0.616470546886727</v>
-      </c>
-      <c r="I12" s="38">
-        <v>0.018014897258063</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>8</v>
@@ -10900,86 +10910,86 @@
       <c r="A16" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="40">
         <v>0.646754816821959</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="39">
         <v>0.01567039872775</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="39">
         <v>0.662679680050151</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="39">
         <v>0.011552184683067</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="39">
         <v>0.669639018764573</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="39">
         <v>0.008673767879664</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="40">
         <v>0.677762757672282</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="39">
         <v>0.006638033701574</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="40">
+        <v>27</v>
+      </c>
+      <c r="B17" s="41">
         <v>0.462357092508698</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="41">
         <v>0.006789716206943</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="41">
         <v>0.47531016238187</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="41">
         <v>0.004598834765242</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="41">
         <v>0.48099700947667</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="41">
         <v>0.004599164036628</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="41">
         <v>0.488012417122804</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="41">
         <v>0.00441587636963</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="40">
+        <v>28</v>
+      </c>
+      <c r="B18" s="41">
         <v>0.499317365397346</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="41">
         <v>0.002609154936188</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="41">
         <v>0.498326629044775</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="41">
         <v>0.003123896642822</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="41">
         <v>0.498228686986251</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="41">
         <v>0.002823312965213</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="41">
         <v>0.497361777137967</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="41">
         <v>0.003339699814354</v>
       </c>
     </row>
@@ -10987,62 +10997,62 @@
       <c r="A19" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="39">
         <v>0.567448620972711</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="39">
         <v>0.009067587700013</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="39">
         <v>0.569274598531765</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="39">
         <v>0.010295122757525</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="39">
         <v>0.57072785472177</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="39">
         <v>0.007117781483861</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="39">
         <v>0.571279380524076</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="39">
         <v>0.00492011233907</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="38">
+      <c r="A20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="39">
         <v>0.436495352293074</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="39">
         <v>0.072485955542141</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="39">
         <v>0.470144313787286</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="39">
         <v>0.099938124940213</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="39">
         <v>0.492697576527756</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="39">
         <v>0.025462428522499</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="39">
         <v>0.4937587668161</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="39">
         <v>0.029271047022238</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="16">
@@ -11072,30 +11082,30 @@
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="38">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39">
         <v>0.578058306872364</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="39">
         <v>0.010241322586894</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="39">
         <v>0.582698250884505</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="39">
         <v>0.013101730911153</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="39">
         <v>0.590921061982592</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="39">
         <v>0.006069759944119</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="39">
         <v>0.585168536787222</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="39">
         <v>0.006674219812666</v>
       </c>
     </row>
@@ -11103,114 +11113,114 @@
       <c r="A23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="39">
         <v>0.564411571684472</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>0.014741359914966</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="39">
         <v>0.572862986418112</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="39">
         <v>0.012030822838234</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="39">
         <v>0.571038279473281</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="39">
         <v>0.008984542352852</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="39">
         <v>0.568596285764833</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="39">
         <v>0.008044377899667</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="38">
+        <v>23</v>
+      </c>
+      <c r="B24" s="39">
         <v>0.645510587545256</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="39">
         <v>0.044139453247141</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="40">
         <v>0.671100042501942</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="39">
         <v>0.055104468410046</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="40">
         <v>0.681238356103717</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="39">
         <v>0.018187571194276</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="39">
         <v>0.673382612068842</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="39">
         <v>0.025886825722313</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="38">
+        <v>24</v>
+      </c>
+      <c r="B25" s="39">
         <v>0.610103855051617</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="39">
         <v>0.00858759076774</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="39">
         <v>0.615196131242253</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="39">
         <v>0.007954610544378</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="39">
         <v>0.611911071117249</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="39">
         <v>0.005887569441382</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="39">
         <v>0.613056213334011</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="39">
         <v>0.003435657693186</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="33"/>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
+      <c r="A28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>8</v>
@@ -11260,86 +11270,86 @@
       <c r="A30" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="39">
         <v>0.863352397032499</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="39">
         <v>0.014716228612674</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="39">
         <v>0.856782794587483</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="39">
         <v>0.010823759655585</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="39">
         <v>0.852748846512525</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="39">
         <v>0.009597695332687</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="39">
         <v>0.85218812619875</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="39">
         <v>0.008737941926615</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="40">
+        <v>27</v>
+      </c>
+      <c r="B31" s="41">
         <v>0.548322398471998</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="41">
         <v>0.018325305645241</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="41">
         <v>0.55926509074842</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="41">
         <v>0.010756372193032</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="41">
         <v>0.5669142315141</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="41">
         <v>0.014134997608064</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="41">
         <v>0.567329023499822</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="41">
         <v>0.014314658884795</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="40">
+        <v>28</v>
+      </c>
+      <c r="B32" s="41">
         <v>0.528128232375133</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="41">
         <v>0.02061347512628</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="41">
         <v>0.554647984168176</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="41">
         <v>0.010175653315936</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="41">
         <v>0.56563198751279</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="41">
         <v>0.00951817176553</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="41">
         <v>0.576491735542698</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="41">
         <v>0.007417988955411</v>
       </c>
     </row>
@@ -11347,62 +11357,62 @@
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="39">
         <v>0.852095362702668</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="39">
         <v>0.015182580198316</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="39">
         <v>0.859099161602873</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="39">
         <v>0.010457150652877</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="39">
         <v>0.862023469277136</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="39">
         <v>0.006950033864786</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="39">
         <v>0.865302566928931</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="39">
         <v>0.008743340814991</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="38">
+      <c r="A34" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="39">
         <v>0.514737639856885</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="39">
         <v>0.058373124988492</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="39">
         <v>0.568386724530974</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="39">
         <v>0.076322959189153</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="39">
         <v>0.542808405008391</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="39">
         <v>0.082023857743016</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="39">
         <v>0.592058362689784</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="39">
         <v>0.064118002265851</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="16">
@@ -11432,30 +11442,30 @@
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="38">
+        <v>22</v>
+      </c>
+      <c r="B36" s="39">
         <v>0.816319794489295</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="39">
         <v>0.016388405251883</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="39">
         <v>0.823543094447576</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="39">
         <v>0.017232254432468</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="39">
         <v>0.824553369316367</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="39">
         <v>0.010098787988353</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="39">
         <v>0.82730508760729</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="39">
         <v>0.017286744449277</v>
       </c>
     </row>
@@ -11463,86 +11473,86 @@
       <c r="A37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="39">
         <v>0.887884200520441</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="39">
         <v>0.019785286177768</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="39">
         <v>0.895295006337795</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="39">
         <v>0.014189979690871</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="39">
         <v>0.894066126876736</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="39">
         <v>0.011942097085339</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="39">
         <v>0.896100667856475</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="39">
         <v>0.017697136427147</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="39">
+        <v>23</v>
+      </c>
+      <c r="B38" s="40">
         <v>0.908826651769629</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="39">
         <v>0.01810208289458</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="40">
         <v>0.906284921736125</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="39">
         <v>0.015033530128245</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="40">
         <v>0.901693102022718</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="39">
         <v>0.013858315088995</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="40">
         <v>0.902542635829398</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="39">
         <v>0.012150335607389</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="38">
+        <v>24</v>
+      </c>
+      <c r="B39" s="39">
         <v>0.79678126450884</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="39">
         <v>0.032046735286035</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="39">
         <v>0.799134316979913</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="39">
         <v>0.021970392511908</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="39">
         <v>0.8103299098025</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="39">
         <v>0.032684361359298</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="39">
         <v>0.809701126396903</v>
       </c>
-      <c r="I39" s="38">
+      <c r="I39" s="39">
         <v>0.029959801985247</v>
       </c>
     </row>
@@ -11579,7 +11589,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -11600,7 +11610,7 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
@@ -11630,86 +11640,86 @@
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="38">
         <v>0.529153624741568</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="38">
         <v>9.81972020478E-4</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="38">
         <v>0.535355919709583</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="38">
         <v>0.002438666571176</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="38">
         <v>0.542421134170567</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="38">
         <v>0.002644662071412</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="38">
         <v>0.548038355819234</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="38">
         <v>0.003040874631307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="40">
+        <v>27</v>
+      </c>
+      <c r="B4" s="41">
         <v>0.515037603878596</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="41">
         <v>0.002501899485345</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="41">
         <v>0.515973806773508</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="41">
         <v>0.002096179238687</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="41">
         <v>0.518255838772836</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="41">
         <v>0.002428618937852</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="41">
         <v>0.519104236808068</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="41">
         <v>0.001700151473056</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="40">
+        <v>28</v>
+      </c>
+      <c r="B5" s="41">
         <v>0.509639853726749</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="41">
         <v>0.002640140918611</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="41">
         <v>0.511263606030348</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="41">
         <v>0.002002983007681</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="41">
         <v>0.512433829694603</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="41">
         <v>0.002741642016495</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="41">
         <v>0.515622734967114</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="41">
         <v>0.002084390388252</v>
       </c>
     </row>
@@ -11717,62 +11727,62 @@
       <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="39">
         <v>0.572642562116621</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="39">
         <v>0.004260944522355</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="39">
         <v>0.571165092050252</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="39">
         <v>0.004795645451604</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="39">
         <v>0.571165130563032</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="39">
         <v>0.004400277706585</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="39">
         <v>0.570667904895342</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="39">
         <v>0.003048749123833</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="38">
+      <c r="A7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39">
         <v>0.545170563689312</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="39">
         <v>0.024533123464399</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="39">
         <v>0.555907854065319</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="39">
         <v>0.019551877673234</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="39">
         <v>0.559096551796737</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="39">
         <v>0.024960142105917</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="39">
         <v>0.559155285926155</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="39">
         <v>0.017580639377736</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="16">
@@ -11802,30 +11812,30 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="38">
+        <v>22</v>
+      </c>
+      <c r="B9" s="39">
         <v>0.566074539089744</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="39">
         <v>0.007092672918018</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="39">
         <v>0.57230604172235</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="39">
         <v>0.006058270589529</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="39">
         <v>0.573695739023023</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="39">
         <v>0.00940357082993</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="39">
         <v>0.57340341632324</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="39">
         <v>0.005771159431586</v>
       </c>
     </row>
@@ -11833,103 +11843,103 @@
       <c r="A10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="39">
         <v>0.570609282025067</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="39">
         <v>0.007428902487432</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="39">
         <v>0.567361743184286</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="39">
         <v>0.004828651905158</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="39">
         <v>0.568371126780392</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="39">
         <v>0.006712447367708</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="39">
         <v>0.568766139529406</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="39">
         <v>0.004554347820204</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="38">
+        <v>23</v>
+      </c>
+      <c r="B11" s="39">
         <v>0.586334602201065</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="39">
         <v>0.01448956829503</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="40">
         <v>0.592404982338467</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="39">
         <v>0.007523110665007</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="40">
         <v>0.598534203585232</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="39">
         <v>0.010207995036188</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="40">
         <v>0.60103496678016</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="39">
         <v>0.016636495450048</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="40">
+        <v>0.590152196516511</v>
+      </c>
+      <c r="C12" s="39">
+        <v>0.010480397913063</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0.587958059240016</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.010341903240206</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.583379377501672</v>
+      </c>
+      <c r="G12" s="39">
+        <v>0.007681183359739</v>
+      </c>
+      <c r="H12" s="39">
+        <v>0.578010890643988</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.008622348902459</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="32" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="39">
-        <v>0.590152196516511</v>
-      </c>
-      <c r="C12" s="38">
-        <v>0.010480397913063</v>
-      </c>
-      <c r="D12" s="38">
-        <v>0.587958059240016</v>
-      </c>
-      <c r="E12" s="38">
-        <v>0.010341903240206</v>
-      </c>
-      <c r="F12" s="38">
-        <v>0.583379377501672</v>
-      </c>
-      <c r="G12" s="38">
-        <v>0.007681183359739</v>
-      </c>
-      <c r="H12" s="38">
-        <v>0.578010890643988</v>
-      </c>
-      <c r="I12" s="38">
-        <v>0.008622348902459</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>8</v>
@@ -11979,86 +11989,86 @@
       <c r="A16" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="39">
         <v>0.775484820445345</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="39">
         <v>1.65457876162E-4</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="40">
         <v>0.776084890415058</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="39">
         <v>8.04776811126E-4</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="40">
         <v>0.776728897097054</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="39">
         <v>0.001375011671421</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="40">
         <v>0.778089990509619</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="39">
         <v>0.002039383471413</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="40">
+        <v>27</v>
+      </c>
+      <c r="B17" s="41">
         <v>0.586344705025309</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="41">
         <v>0.021478006991606</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="41">
         <v>0.608620924474182</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="41">
         <v>0.020456390452307</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="41">
         <v>0.623988740154458</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="41">
         <v>0.016621568051996</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="41">
         <v>0.642400291874637</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="41">
         <v>0.011490590922756</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="40">
+        <v>28</v>
+      </c>
+      <c r="B18" s="41">
         <v>0.538191824888242</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="41">
         <v>0.023241780475049</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="41">
         <v>0.602136145499986</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="41">
         <v>0.030871141752211</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="41">
         <v>0.641155609007259</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="41">
         <v>0.026416672863225</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="41">
         <v>0.673618717249359</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="41">
         <v>0.014565466760996</v>
       </c>
     </row>
@@ -12066,62 +12076,62 @@
       <c r="A19" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="39">
         <v>0.759971273088891</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="39">
         <v>0.009046697651347</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="39">
         <v>0.755975519254781</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="39">
         <v>0.008918755109435</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="39">
         <v>0.755858476788666</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="39">
         <v>0.008849891406377</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="39">
         <v>0.758902409902214</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="39">
         <v>0.005068257197306</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="38">
+      <c r="A20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="39">
         <v>0.59986778714744</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="39">
         <v>0.073858626946475</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="39">
         <v>0.644418664450759</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="39">
         <v>0.042728661536537</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="39">
         <v>0.664911515218712</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="39">
         <v>0.053012405329025</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="39">
         <v>0.664587740357015</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="39">
         <v>0.032095605572053</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="16">
@@ -12151,30 +12161,30 @@
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="38">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39">
         <v>0.775543400586286</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="39">
         <v>7.04282502907E-4</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="39">
         <v>0.775528729310266</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="39">
         <v>6.28946035533E-4</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="39">
         <v>0.774884774038786</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="39">
         <v>0.00148827340697</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="39">
         <v>0.774328550812954</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="39">
         <v>0.001154430364064</v>
       </c>
     </row>
@@ -12182,116 +12192,116 @@
       <c r="A23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="39">
         <v>0.758141122980466</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>0.007742564616662</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="39">
         <v>0.763073709227605</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="39">
         <v>0.005048733196666</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="39">
         <v>0.764698300813897</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="39">
         <v>0.005527201355746</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="39">
         <v>0.76283944007436</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="39">
         <v>0.004312313744229</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="38">
+        <v>23</v>
+      </c>
+      <c r="B24" s="39">
         <v>0.773245628992241</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="39">
         <v>0.002411255654385</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="39">
         <v>0.775162834241186</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="39">
         <v>0.001009281815969</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="39">
         <v>0.774957944055762</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="39">
         <v>0.001013588228102</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="39">
         <v>0.774796926319477</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="39">
         <v>7.11012230953E-4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="39">
+        <v>24</v>
+      </c>
+      <c r="B25" s="40">
         <v>0.775587260182795</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="39">
         <v>4.51938576699E-4</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="39">
         <v>0.775923894099821</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="39">
         <v>8.75292689417E-4</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="39">
         <v>0.775558014025474</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="39">
         <v>5.16121140253E-4</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="39">
         <v>0.775587255898586</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="39">
         <v>5.11714906591E-4</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="33"/>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
+      <c r="A28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>8</v>
@@ -12341,86 +12351,86 @@
       <c r="A30" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="39">
         <v>0.520565443635341</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="39">
         <v>1.71818667308E-4</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="39">
         <v>0.52296392370118</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="39">
         <v>0.001281870214316</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="39">
         <v>0.528985738246294</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="39">
         <v>0.002344757138974</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="39">
         <v>0.546234386557073</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="39">
         <v>0.005803442844759</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="40">
+        <v>27</v>
+      </c>
+      <c r="B31" s="41">
         <v>0.558991702347095</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="41">
         <v>0.01210931062329</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="41">
         <v>0.568637189944891</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="41">
         <v>0.006995635504715</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="41">
         <v>0.572158249210863</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="41">
         <v>0.005964097075387</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="41">
         <v>0.575066725005469</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="41">
         <v>0.006448977680015</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="40">
+        <v>28</v>
+      </c>
+      <c r="B32" s="41">
         <v>0.551745007344439</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="41">
         <v>0.019156996539389</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="41">
         <v>0.568738866143701</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="41">
         <v>0.00780695866348</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="41">
         <v>0.574250398474857</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="41">
         <v>0.010302925620714</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="41">
         <v>0.583588904168099</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="41">
         <v>0.008088123770614</v>
       </c>
     </row>
@@ -12428,62 +12438,62 @@
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="39">
         <v>0.64288678105239</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="39">
         <v>0.02075963638728</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="39">
         <v>0.697389390672042</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="39">
         <v>0.018768374572908</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="39">
         <v>0.728159827483827</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="39">
         <v>0.011838660479109</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="39">
         <v>0.759493259784771</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="39">
         <v>0.011158501847143</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="38">
+      <c r="A34" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="39">
         <v>0.525872295319353</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="39">
         <v>0.019322591167912</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="39">
         <v>0.557565500932379</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="39">
         <v>0.058101342110684</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="39">
         <v>0.538420294610953</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="39">
         <v>0.046353414496788</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="39">
         <v>0.572818597576856</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="39">
         <v>0.034472582481974</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="16">
@@ -12513,30 +12523,30 @@
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="38">
+        <v>22</v>
+      </c>
+      <c r="B36" s="39">
         <v>0.616403881613901</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="39">
         <v>0.022678228871418</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="39">
         <v>0.688917476638435</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="39">
         <v>0.017225440896575</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="39">
         <v>0.72652628892292</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="39">
         <v>0.009136224893396</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="39">
         <v>0.746024340823619</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="39">
         <v>0.02091884103943</v>
       </c>
     </row>
@@ -12544,86 +12554,86 @@
       <c r="A37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="39">
         <v>0.776999692679522</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="39">
         <v>0.025488805588706</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="39">
         <v>0.799955464574804</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="39">
         <v>0.03157603292751</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="39">
         <v>0.798684147472159</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="39">
         <v>0.019165234756159</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="39">
         <v>0.803629975726891</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="39">
         <v>0.02064040259462</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="39">
+        <v>23</v>
+      </c>
+      <c r="B38" s="40">
         <v>0.815573491264806</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="39">
         <v>0.019975322297748</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="40">
         <v>0.816800429206905</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="39">
         <v>0.025747827609362</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="40">
         <v>0.80965262368347</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="39">
         <v>0.035726734963609</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="40">
         <v>0.80567495911075</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="39">
         <v>0.007379340396246</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="38">
+        <v>24</v>
+      </c>
+      <c r="B39" s="39">
         <v>0.728669901344918</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="39">
         <v>0.012489999281487</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="39">
         <v>0.733875493535852</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="39">
         <v>0.018710055530801</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="39">
         <v>0.733362580866956</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="39">
         <v>0.013424656986936</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="39">
         <v>0.73642536800325</v>
       </c>
-      <c r="I39" s="38">
+      <c r="I39" s="39">
         <v>0.023209089171926</v>
       </c>
     </row>

</xml_diff>